<commit_message>
Added music and updated credits
</commit_message>
<xml_diff>
--- a/Writing/Good Boy Credits.xlsx
+++ b/Writing/Good Boy Credits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Credits</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Alexander Liavas</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Bensound</t>
+  </si>
+  <si>
+    <t>Purple Planet Music</t>
   </si>
 </sst>
 </file>
@@ -422,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,6 +577,24 @@
         <v>26</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Credits and started responsibilities document
</commit_message>
<xml_diff>
--- a/Writing/Good Boy Credits.xlsx
+++ b/Writing/Good Boy Credits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Credits</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Alex Francoletti</t>
   </si>
   <si>
-    <t>Kevin</t>
-  </si>
-  <si>
     <t>Level Design</t>
   </si>
   <si>
@@ -107,16 +104,19 @@
     <t>Alexander Liavas</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>Sources</t>
-  </si>
-  <si>
     <t>Bensound</t>
   </si>
   <si>
     <t>Purple Planet Music</t>
+  </si>
+  <si>
+    <t>Kevin Chen</t>
+  </si>
+  <si>
+    <t>Music (Selection)</t>
+  </si>
+  <si>
+    <t>Music (Sources)</t>
   </si>
 </sst>
 </file>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,17 +537,17 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -571,28 +571,31 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>